<commit_message>
Update Planemo Module Support.xlsx
</commit_message>
<xml_diff>
--- a/Planemo Module Support.xlsx
+++ b/Planemo Module Support.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10701"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/profmc/Library/CloudStorage/Dropbox/WorldCrafting101-DEV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CA69B9-9AC3-6F4A-9CBD-DBDA61C4FFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A40190-01FF-B844-9757-04007C1502F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15000" yWindow="23060" windowWidth="33720" windowHeight="16940" xr2:uid="{A45E239F-017E-8B4E-B0E1-84F8677CA5DA}"/>
+    <workbookView xWindow="-12500" yWindow="23060" windowWidth="33720" windowHeight="16940" xr2:uid="{A45E239F-017E-8B4E-B0E1-84F8677CA5DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -273,9 +273,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="174" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -312,12 +313,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="174" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,26 +689,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B438628E-6319-1A4C-A2C5-CDA6E93202CA}">
-  <dimension ref="A2:N24"/>
+  <dimension ref="A2:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:D12"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.5703125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="5.5703125" style="1"/>
+    <col min="11" max="11" width="5.5703125" style="1"/>
+    <col min="12" max="13" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="5.5703125" style="1"/>
+    <col min="16" max="16" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.5703125" style="1"/>
+    <col min="18" max="18" width="11.42578125" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="5.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:18">
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
@@ -711,7 +722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:18">
       <c r="C3" s="1">
         <v>0.5</v>
       </c>
@@ -730,7 +741,7 @@
         <v>3.375</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:18">
       <c r="E4" s="1" t="str">
         <v>R</v>
       </c>
@@ -742,7 +753,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:18">
       <c r="E5" s="1" t="str">
         <v>d ➔</v>
       </c>
@@ -750,7 +761,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:18">
       <c r="E6" s="1" t="str">
         <v>g ➔</v>
       </c>
@@ -758,7 +769,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:18">
       <c r="E7" s="1" t="str">
         <v>v</v>
       </c>
@@ -766,7 +777,7 @@
         <v>2.1213199999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:18">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -791,12 +802,15 @@
       <c r="N9" s="1">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="C10" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="D10" s="1">
+      <c r="R9" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="C10" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="4">
         <v>1.5</v>
       </c>
       <c r="I10" s="1">
@@ -811,21 +825,29 @@
       <c r="N10" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="R10" s="1" cm="1">
+        <f t="array" ref="R10">General.ROOT(0.5)</f>
+        <v>0.70710678118654757</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="C11" s="2">
+      <c r="B11" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="4">
         <f>$B11^3/C$10^2</f>
         <v>0.5</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="6">
         <f>$B11^3/D$10^2</f>
         <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="E11" s="4">
+        <f>0.5-D11</f>
+        <v>0.44444444444444442</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>4</v>
@@ -849,19 +871,23 @@
         <f>N9^3/N10^2</f>
         <v>8.788000000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="R11" s="1">
+        <f>R9/R10</f>
+        <v>2.1213203435596424</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="C12" s="2">
+      <c r="B12" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="C12" s="4">
         <f>$B12^3/C$10^2</f>
         <v>13.5</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="4">
         <f>$B12^3/D$10^2</f>
         <v>1.5</v>
       </c>
@@ -881,10 +907,10 @@
       </c>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:18">
       <c r="L13" s="3"/>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:18">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -894,16 +920,28 @@
       <c r="D15" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="O15" s="1">
+        <f>1.5/0.25</f>
+        <v>6</v>
+      </c>
+      <c r="P15" s="5" cm="1">
+        <f t="array" ref="P15">General.ROOT(O15,3)</f>
+        <v>1.8171205928321397</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="C16" s="1">
         <v>0.5</v>
       </c>
       <c r="D16" s="1">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="K16" s="1">
+        <f>0.7^3/0.5^2</f>
+        <v>1.3719999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -918,8 +956,23 @@
         <f>$B17/D$16</f>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="N17" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="O17" s="1">
+        <f>0.5^2</f>
+        <v>0.25</v>
+      </c>
+      <c r="P17" s="1">
+        <f>N17*O17</f>
+        <v>0.125</v>
+      </c>
+      <c r="Q17" s="1" cm="1">
+        <f t="array" ref="Q17">General.ROOT(P17,3)</f>
+        <v>0.50000000000000011</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
@@ -935,8 +988,28 @@
         <v>1</v>
       </c>
       <c r="L18" s="4"/>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="P18" s="1">
+        <f>P17^(1/3)</f>
+        <v>0.50000000000000011</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="L19" s="1">
+        <f>1.5^3</f>
+        <v>3.375</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="L20" s="6">
+        <f>L19/0.5</f>
+        <v>6.75</v>
+      </c>
+      <c r="M20" s="6" cm="1">
+        <f t="array" ref="M20">General.ROOT(L20)</f>
+        <v>2.598076211353316</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -946,8 +1019,12 @@
       <c r="D21" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="M21" s="6">
+        <f>M20-1.5</f>
+        <v>1.098076211353316</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
       <c r="C22" s="1">
         <v>0.5</v>
       </c>
@@ -955,7 +1032,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:17">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
@@ -970,8 +1047,12 @@
         <f>$B23/SQRT(D$22)</f>
         <v>0.40824829046386307</v>
       </c>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="M23" s="1">
+        <f>2.6*5.514</f>
+        <v>14.336400000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
       <c r="A24" s="1" t="s">
         <v>3</v>
       </c>

</xml_diff>